<commit_message>
Updated Lookup with Bar Chart
</commit_message>
<xml_diff>
--- a/metro_budget_exercise.xlsx
+++ b/metro_budget_exercise.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/384aa62402beba2a/Documents/DA15/Excel/lookups-exercise-mbainbridge950/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malan\OneDrive\Documents\DA15\Excel\lookups-exercise-mbainbridge950\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="168" documentId="8_{19ED61FC-0AAB-4DAC-83F6-00D6AC42053B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{940F8D88-D763-418A-8A1B-55A2F15511F5}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAEB99E2-D9D7-4EF9-A03D-F687BBBEFC60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="972" yWindow="924" windowWidth="21600" windowHeight="11232" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31995" yWindow="1665" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="metro_budget" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -901,6 +901,997 @@
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Department</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Budget Vs Actual</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metro_budget!$B$83</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Budget</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>metro_budget!$A$84:$A$86</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>FY17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$B$84:$B$86</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>9349400</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11073700</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10790500</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-78B4-4A20-B00D-F6E80E439AC2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>metro_budget!$C$83</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>metro_budget!$A$84:$A$86</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>FY17</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FY18</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>FY19</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>metro_budget!$C$84:$C$86</c:f>
+              <c:numCache>
+                <c:formatCode>_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* "-"??_);_(@_)</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>8952825.2799999993</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>9929059.5199999996</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>9929059.5199999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-78B4-4A20-B00D-F6E80E439AC2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1125404527"/>
+        <c:axId val="1125406447"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1125404527"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1125406447"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1125406447"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1125404527"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>948690</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>18097</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>112395</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>50482</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4D4B7B87-7101-84EF-4A64-A24F30056191}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -1200,8 +2191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G31" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P52"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="B87" sqref="B87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1288,7 +2279,7 @@
         <v>-4.3170750765267295E-2</v>
       </c>
       <c r="F2">
-        <f>IFERROR(RANK(E2,E2:E52)," ")</f>
+        <f>IFERROR(RANK(E2,$E$2:$E$52)," ")</f>
         <v>35</v>
       </c>
       <c r="G2">
@@ -1306,7 +2297,7 @@
         <v>-9.4972027086493035E-2</v>
       </c>
       <c r="K2">
-        <f>IFERROR(RANK(J2, J2:J52), " ")</f>
+        <f>IFERROR(RANK(J2, $J$2:$J$52), " ")</f>
         <v>39</v>
       </c>
       <c r="L2">
@@ -1324,7 +2315,7 @@
         <v>-5.6484362894991494E-2</v>
       </c>
       <c r="P2">
-        <f>IFERROR(RANK(O2, O2:O52), " ")</f>
+        <f>IFERROR(RANK(O2, $O$2:$O$52), " ")</f>
         <v>35</v>
       </c>
     </row>
@@ -1347,7 +2338,7 @@
         <v>-2.3069981751824741E-2</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F52" si="2">IFERROR(RANK(E3,E3:E53)," ")</f>
+        <f t="shared" ref="F3:F52" si="2">IFERROR(RANK(E3,$E$2:$E$52)," ")</f>
         <v>27</v>
       </c>
       <c r="G3">
@@ -1365,7 +2356,7 @@
         <v>-6.6804928315415249E-2</v>
       </c>
       <c r="K3">
-        <f t="shared" ref="K3:K52" si="5">IFERROR(RANK(J3, J3:J53), " ")</f>
+        <f t="shared" ref="K3:K52" si="5">IFERROR(RANK(J3, $J$2:$J$52), " ")</f>
         <v>35</v>
       </c>
       <c r="L3">
@@ -1383,7 +2374,7 @@
         <v>-1.3540749922529313E-3</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P52" si="8">IFERROR(RANK(O3, O3:O53), " ")</f>
+        <f t="shared" ref="P3:P52" si="8">IFERROR(RANK(O3, $O$2:$O$52), " ")</f>
         <v>12</v>
       </c>
     </row>
@@ -1443,7 +2434,7 @@
       </c>
       <c r="P4">
         <f t="shared" si="8"/>
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.3">
@@ -1466,7 +2457,7 @@
       </c>
       <c r="F5">
         <f t="shared" si="2"/>
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="G5">
         <v>7968300</v>
@@ -1484,7 +2475,7 @@
       </c>
       <c r="K5">
         <f t="shared" si="5"/>
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="L5">
         <v>7759600</v>
@@ -1502,7 +2493,7 @@
       </c>
       <c r="P5">
         <f t="shared" si="8"/>
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.3">
@@ -1525,7 +2516,7 @@
       </c>
       <c r="F6">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="G6">
         <v>428500</v>
@@ -1584,7 +2575,7 @@
       </c>
       <c r="F7">
         <f t="shared" si="2"/>
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="G7">
         <v>3390900</v>
@@ -1602,7 +2593,7 @@
       </c>
       <c r="K7">
         <f t="shared" si="5"/>
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="L7">
         <v>3345200</v>
@@ -1620,7 +2611,7 @@
       </c>
       <c r="P7">
         <f t="shared" si="8"/>
-        <v>40</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.3">
@@ -1643,7 +2634,7 @@
       </c>
       <c r="F8">
         <f t="shared" si="2"/>
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="G8">
         <v>1590700</v>
@@ -1661,7 +2652,7 @@
       </c>
       <c r="K8">
         <f t="shared" si="5"/>
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="L8">
         <v>1579300</v>
@@ -1679,7 +2670,7 @@
       </c>
       <c r="P8">
         <f t="shared" si="8"/>
-        <v>41</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
@@ -1702,7 +2693,7 @@
       </c>
       <c r="F9">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G9">
         <v>11073700</v>
@@ -1720,7 +2711,7 @@
       </c>
       <c r="K9">
         <f t="shared" si="5"/>
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="L9">
         <v>10790500</v>
@@ -1738,7 +2729,7 @@
       </c>
       <c r="P9">
         <f t="shared" si="8"/>
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
@@ -1761,7 +2752,7 @@
       </c>
       <c r="F10">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="G10">
         <v>495200</v>
@@ -1779,7 +2770,7 @@
       </c>
       <c r="K10">
         <f t="shared" si="5"/>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="L10">
         <v>487500</v>
@@ -1797,7 +2788,7 @@
       </c>
       <c r="P10">
         <f t="shared" si="8"/>
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.3">
@@ -1856,7 +2847,7 @@
       </c>
       <c r="P11">
         <f t="shared" si="8"/>
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.3">
@@ -1879,7 +2870,7 @@
       </c>
       <c r="F12">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="G12">
         <v>4700400</v>
@@ -1897,7 +2888,7 @@
       </c>
       <c r="K12">
         <f t="shared" si="5"/>
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="L12">
         <v>4677800</v>
@@ -1915,7 +2906,7 @@
       </c>
       <c r="P12">
         <f t="shared" si="8"/>
-        <v>33</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.3">
@@ -1938,7 +2929,7 @@
       </c>
       <c r="F13">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G13">
         <v>6223700</v>
@@ -1956,7 +2947,7 @@
       </c>
       <c r="K13">
         <f t="shared" si="5"/>
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="L13">
         <v>6207300</v>
@@ -1974,7 +2965,7 @@
       </c>
       <c r="P13">
         <f t="shared" si="8"/>
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.3">
@@ -1997,7 +2988,7 @@
       </c>
       <c r="F14">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="G14">
         <v>530500</v>
@@ -2015,7 +3006,7 @@
       </c>
       <c r="K14">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L14">
         <v>526200</v>
@@ -2033,7 +3024,7 @@
       </c>
       <c r="P14">
         <f t="shared" si="8"/>
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.3">
@@ -2074,7 +3065,7 @@
       </c>
       <c r="K15">
         <f t="shared" si="5"/>
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="L15">
         <v>188953500</v>
@@ -2092,7 +3083,7 @@
       </c>
       <c r="P15">
         <f t="shared" si="8"/>
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.3">
@@ -2115,7 +3106,7 @@
       </c>
       <c r="F16">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="G16">
         <v>7352500</v>
@@ -2174,7 +3165,7 @@
       </c>
       <c r="F17">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G17">
         <v>15309700</v>
@@ -2192,7 +3183,7 @@
       </c>
       <c r="K17">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="L17">
         <v>15311800</v>
@@ -2210,7 +3201,7 @@
       </c>
       <c r="P17">
         <f t="shared" si="8"/>
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.3">
@@ -2233,7 +3224,7 @@
       </c>
       <c r="F18">
         <f t="shared" si="2"/>
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="G18">
         <v>2861000</v>
@@ -2251,7 +3242,7 @@
       </c>
       <c r="K18">
         <f t="shared" si="5"/>
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="L18">
         <v>2910600</v>
@@ -2269,7 +3260,7 @@
       </c>
       <c r="P18">
         <f t="shared" si="8"/>
-        <v>32</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.3">
@@ -2292,7 +3283,7 @@
       </c>
       <c r="F19">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="G19">
         <v>9713300</v>
@@ -2310,7 +3301,7 @@
       </c>
       <c r="K19">
         <f t="shared" si="5"/>
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="L19">
         <v>9343000</v>
@@ -2328,7 +3319,7 @@
       </c>
       <c r="P19">
         <f t="shared" si="8"/>
-        <v>27</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.3">
@@ -2351,7 +3342,7 @@
       </c>
       <c r="F20">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G20">
         <v>131849400</v>
@@ -2410,7 +3401,7 @@
       </c>
       <c r="F21">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="G21">
         <v>24497400</v>
@@ -2428,7 +3419,7 @@
       </c>
       <c r="K21">
         <f t="shared" si="5"/>
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="L21">
         <v>24323000</v>
@@ -2446,7 +3437,7 @@
       </c>
       <c r="P21">
         <f t="shared" si="8"/>
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.3">
@@ -2469,7 +3460,7 @@
       </c>
       <c r="F22">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="G22">
         <v>11980700</v>
@@ -2487,7 +3478,7 @@
       </c>
       <c r="K22">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="L22">
         <v>11935200</v>
@@ -2505,7 +3496,7 @@
       </c>
       <c r="P22">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.3">
@@ -2528,7 +3519,7 @@
       </c>
       <c r="F23">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="G23">
         <v>22683800</v>
@@ -2546,7 +3537,7 @@
       </c>
       <c r="K23">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="L23">
         <v>23220300</v>
@@ -2564,7 +3555,7 @@
       </c>
       <c r="P23">
         <f t="shared" si="8"/>
-        <v>15</v>
+        <v>23</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.3">
@@ -2587,7 +3578,7 @@
       </c>
       <c r="F24">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G24">
         <v>1112700</v>
@@ -2605,7 +3596,7 @@
       </c>
       <c r="K24">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="L24">
         <v>1112600</v>
@@ -2623,7 +3614,7 @@
       </c>
       <c r="P24">
         <f t="shared" si="8"/>
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.3">
@@ -2646,7 +3637,7 @@
       </c>
       <c r="F25">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="G25">
         <v>505200</v>
@@ -2664,7 +3655,7 @@
       </c>
       <c r="K25">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="L25">
         <v>496500</v>
@@ -2682,7 +3673,7 @@
       </c>
       <c r="P25">
         <f t="shared" si="8"/>
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.3">
@@ -2705,7 +3696,7 @@
       </c>
       <c r="F26">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="G26">
         <v>5442200</v>
@@ -2723,7 +3714,7 @@
       </c>
       <c r="K26">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="L26">
         <v>5430700</v>
@@ -2741,7 +3732,7 @@
       </c>
       <c r="P26">
         <f t="shared" si="8"/>
-        <v>20</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.3">
@@ -2823,7 +3814,7 @@
       </c>
       <c r="F28">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="G28">
         <v>1545700</v>
@@ -2841,7 +3832,7 @@
       </c>
       <c r="K28">
         <f t="shared" si="5"/>
-        <v>23</v>
+        <v>47</v>
       </c>
       <c r="L28">
         <v>1525900</v>
@@ -2859,7 +3850,7 @@
       </c>
       <c r="P28">
         <f t="shared" si="8"/>
-        <v>21</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.3">
@@ -2882,7 +3873,7 @@
       </c>
       <c r="F29">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="G29">
         <v>2779500</v>
@@ -2900,7 +3891,7 @@
       </c>
       <c r="K29">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="L29">
         <v>2889900</v>
@@ -2918,7 +3909,7 @@
       </c>
       <c r="P29">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.3">
@@ -2941,7 +3932,7 @@
       </c>
       <c r="F30">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="G30">
         <v>12735900</v>
@@ -2959,7 +3950,7 @@
       </c>
       <c r="K30">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="L30">
         <v>12861300</v>
@@ -2977,7 +3968,7 @@
       </c>
       <c r="P30">
         <f t="shared" si="8"/>
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.3">
@@ -3000,7 +3991,7 @@
       </c>
       <c r="F31">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G31">
         <v>1823300</v>
@@ -3018,7 +4009,7 @@
       </c>
       <c r="K31">
         <f t="shared" si="5"/>
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="L31">
         <v>1870700</v>
@@ -3036,7 +4027,7 @@
       </c>
       <c r="P31">
         <f t="shared" si="8"/>
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.3">
@@ -3059,7 +4050,7 @@
       </c>
       <c r="F32">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="G32">
         <v>6195500</v>
@@ -3077,7 +4068,7 @@
       </c>
       <c r="K32">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="L32">
         <v>6157400</v>
@@ -3095,7 +4086,7 @@
       </c>
       <c r="P32">
         <f t="shared" si="8"/>
-        <v>12</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
@@ -3118,7 +4109,7 @@
       </c>
       <c r="F33">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="G33">
         <v>979671000</v>
@@ -3136,7 +4127,7 @@
       </c>
       <c r="K33">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L33">
         <v>989572899.99999905</v>
@@ -3154,7 +4145,7 @@
       </c>
       <c r="P33">
         <f t="shared" si="8"/>
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.3">
@@ -3177,7 +4168,7 @@
       </c>
       <c r="F34">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>23</v>
       </c>
       <c r="G34">
         <v>4350600</v>
@@ -3195,7 +4186,7 @@
       </c>
       <c r="K34">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>28</v>
       </c>
       <c r="L34">
         <v>4345600</v>
@@ -3213,7 +4204,7 @@
       </c>
       <c r="P34">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.3">
@@ -3295,7 +4286,7 @@
       </c>
       <c r="F36">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="G36">
         <v>898700</v>
@@ -3313,7 +4304,7 @@
       </c>
       <c r="K36">
         <f t="shared" si="5"/>
-        <v>17</v>
+        <v>48</v>
       </c>
       <c r="L36">
         <v>878300</v>
@@ -3331,7 +4322,7 @@
       </c>
       <c r="P36">
         <f t="shared" si="8"/>
-        <v>16</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
@@ -3354,7 +4345,7 @@
       </c>
       <c r="F37">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>30</v>
       </c>
       <c r="G37">
         <v>2229200</v>
@@ -3372,7 +4363,7 @@
       </c>
       <c r="K37">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="L37">
         <v>2296900</v>
@@ -3390,7 +4381,7 @@
       </c>
       <c r="P37">
         <f t="shared" si="8"/>
-        <v>14</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
@@ -3413,7 +4404,7 @@
       </c>
       <c r="F38">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="G38">
         <v>792800</v>
@@ -3431,7 +4422,7 @@
       </c>
       <c r="K38">
         <f t="shared" si="5"/>
-        <v>12</v>
+        <v>30</v>
       </c>
       <c r="L38">
         <v>777800</v>
@@ -3449,7 +4440,7 @@
       </c>
       <c r="P38">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.3">
@@ -3472,7 +4463,7 @@
       </c>
       <c r="F39">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="G39">
         <v>1294400</v>
@@ -3490,7 +4481,7 @@
       </c>
       <c r="K39">
         <f t="shared" si="5"/>
-        <v>14</v>
+        <v>46</v>
       </c>
       <c r="L39">
         <v>1759500</v>
@@ -3508,7 +4499,7 @@
       </c>
       <c r="P39">
         <f t="shared" si="8"/>
-        <v>10</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.3">
@@ -3531,7 +4522,7 @@
       </c>
       <c r="F40">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="G40">
         <v>39964900</v>
@@ -3549,7 +4540,7 @@
       </c>
       <c r="K40">
         <f t="shared" si="5"/>
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="L40">
         <v>40216700</v>
@@ -3567,7 +4558,7 @@
       </c>
       <c r="P40">
         <f t="shared" si="8"/>
-        <v>7</v>
+        <v>18</v>
       </c>
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
@@ -3590,7 +4581,7 @@
       </c>
       <c r="F41">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>32</v>
       </c>
       <c r="G41">
         <v>5089500</v>
@@ -3608,7 +4599,7 @@
       </c>
       <c r="K41">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="L41">
         <v>4799900</v>
@@ -3626,7 +4617,7 @@
       </c>
       <c r="P41">
         <f t="shared" si="8"/>
-        <v>7</v>
+        <v>19</v>
       </c>
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.3">
@@ -3649,7 +4640,7 @@
       </c>
       <c r="F42">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G42">
         <v>199130300</v>
@@ -3667,7 +4658,7 @@
       </c>
       <c r="K42">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="L42">
         <v>199954600</v>
@@ -3708,7 +4699,7 @@
       </c>
       <c r="F43">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>25</v>
       </c>
       <c r="G43">
         <v>8560800</v>
@@ -3726,7 +4717,7 @@
       </c>
       <c r="K43">
         <f t="shared" si="5"/>
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="L43">
         <v>8497500</v>
@@ -3744,7 +4735,7 @@
       </c>
       <c r="P43">
         <f t="shared" si="8"/>
-        <v>6</v>
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.3">
@@ -3767,7 +4758,7 @@
       </c>
       <c r="F44">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G44">
         <v>31040700</v>
@@ -3785,7 +4776,7 @@
       </c>
       <c r="K44">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="L44">
         <v>31282200</v>
@@ -3803,7 +4794,7 @@
       </c>
       <c r="P44">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
@@ -3826,7 +4817,7 @@
       </c>
       <c r="F45">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="G45">
         <v>56792200</v>
@@ -3844,7 +4835,7 @@
       </c>
       <c r="K45">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="L45">
         <v>56027100</v>
@@ -3862,7 +4853,7 @@
       </c>
       <c r="P45">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>17</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
@@ -3885,7 +4876,7 @@
       </c>
       <c r="F46">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G46">
         <v>266000</v>
@@ -3903,7 +4894,7 @@
       </c>
       <c r="K46">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="L46">
         <v>267100</v>
@@ -3921,7 +4912,7 @@
       </c>
       <c r="P46">
         <f t="shared" si="8"/>
-        <v>4</v>
+        <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
@@ -3944,7 +4935,7 @@
       </c>
       <c r="F47">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G47">
         <v>73467000</v>
@@ -3962,7 +4953,7 @@
       </c>
       <c r="K47">
         <f t="shared" si="5"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L47">
         <v>75072800</v>
@@ -3980,7 +4971,7 @@
       </c>
       <c r="P47">
         <f t="shared" si="8"/>
-        <v>2</v>
+        <v>11</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
@@ -4003,7 +4994,7 @@
       </c>
       <c r="F48">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="G48">
         <v>7214700</v>
@@ -4021,7 +5012,7 @@
       </c>
       <c r="K48">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="L48">
         <v>7289800</v>
@@ -4039,7 +5030,7 @@
       </c>
       <c r="P48">
         <f t="shared" si="8"/>
-        <v>3</v>
+        <v>34</v>
       </c>
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.3">
@@ -4062,7 +5053,7 @@
       </c>
       <c r="F49">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>22</v>
       </c>
       <c r="G49">
         <v>102600</v>
@@ -4080,7 +5071,7 @@
       </c>
       <c r="K49">
         <f t="shared" si="5"/>
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="L49">
         <v>0</v>
@@ -4121,7 +5112,7 @@
       </c>
       <c r="F50">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G50">
         <v>859100</v>
@@ -4180,7 +5171,7 @@
       </c>
       <c r="F51">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="G51">
         <v>8925500</v>
@@ -4198,7 +5189,7 @@
       </c>
       <c r="K51">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="L51">
         <v>8833900</v>
@@ -4216,7 +5207,7 @@
       </c>
       <c r="P51">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>16</v>
       </c>
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.3">
@@ -4239,7 +5230,7 @@
       </c>
       <c r="F52">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="G52">
         <v>2440700</v>
@@ -4257,7 +5248,7 @@
       </c>
       <c r="K52">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>40</v>
       </c>
       <c r="L52">
         <v>2321600</v>
@@ -4275,7 +5266,7 @@
       </c>
       <c r="P52">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.3">
@@ -4665,11 +5656,11 @@
       </c>
       <c r="B84" s="6">
         <f>INDEX(B2:B52,MATCH(B87, A2:A52))</f>
-        <v>8837300</v>
+        <v>9349400</v>
       </c>
       <c r="C84" s="6">
         <f>INDEX(C2:C52, MATCH(B87, A2:A52))</f>
-        <v>8460963.1999999899</v>
+        <v>8952825.2799999993</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.3">
@@ -4678,11 +5669,11 @@
       </c>
       <c r="B85" s="6">
         <f>INDEX(G2:G52, MATCH(B87, A2:A52))</f>
-        <v>9713300</v>
+        <v>11073700</v>
       </c>
       <c r="C85" s="6">
         <f>INDEX(H2:H52, MATCH(B87, A2:A52))</f>
-        <v>8991707.2399999909</v>
+        <v>9929059.5199999996</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.3">
@@ -4691,16 +5682,16 @@
       </c>
       <c r="B86" s="6">
         <f>INDEX(L2:L52, MATCH(B87, A2:A52))</f>
-        <v>9343000</v>
+        <v>10790500</v>
       </c>
       <c r="C86" s="6">
         <f>INDEX(H2:H52,MATCH(B87,A2:A52))</f>
-        <v>8991707.2399999909</v>
+        <v>9929059.5199999996</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B87" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.3">
@@ -4844,6 +5835,7 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B82:B83" xr:uid="{1248789C-8354-428B-8B98-C97B02054C67}"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>